<commit_message>
Update strokenplanning challange c3.xlsx
</commit_message>
<xml_diff>
--- a/strokenplanning challange c3.xlsx
+++ b/strokenplanning challange c3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikab\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/416185d1c747cde6/Documenten/GitHub/challenge3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{262FDB77-24E1-48A2-A5D3-ECF5E9ED94A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{262FDB77-24E1-48A2-A5D3-ECF5E9ED94A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53EEA756-D7DB-4B84-AA67-DFC24E25F945}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" firstSheet="1" activeTab="1" xr2:uid="{A271F007-5F3A-7D4F-BAC4-1FC3717E9032}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="68">
   <si>
     <t>Strokenplanning</t>
   </si>
@@ -396,10 +396,10 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,10 +737,10 @@
   <dimension ref="A1:BJ60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AQ40" sqref="AQ40"/>
+      <selection pane="bottomRight" activeCell="AQ30" sqref="AQ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -757,96 +757,96 @@
     </row>
     <row r="2" spans="1:62" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A2" s="1"/>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="19" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19" t="s">
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19" t="s">
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19" t="s">
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19" t="s">
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19" t="s">
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19" t="s">
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19" t="s">
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="19"/>
-      <c r="AQ2" s="19" t="s">
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AQ2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="AR2" s="19"/>
-      <c r="AS2" s="19"/>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19" t="s">
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19" t="s">
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19" t="s">
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="20"/>
+      <c r="BB2" s="20"/>
+      <c r="BC2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="19" t="s">
+      <c r="BD2" s="20"/>
+      <c r="BE2" s="20"/>
+      <c r="BF2" s="20"/>
+      <c r="BG2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="BH2" s="19"/>
-      <c r="BI2" s="19"/>
-      <c r="BJ2" s="19"/>
+      <c r="BH2" s="20"/>
+      <c r="BI2" s="20"/>
+      <c r="BJ2" s="20"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
@@ -1661,7 +1661,9 @@
       <c r="AN30" s="16"/>
       <c r="AO30" s="16"/>
       <c r="AP30" s="14"/>
-      <c r="AQ30" s="8"/>
+      <c r="AQ30" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="AR30" s="8"/>
       <c r="AS30" s="8"/>
       <c r="AT30" s="14"/>
@@ -1750,7 +1752,9 @@
       <c r="AJ33" s="16"/>
       <c r="AK33" s="16"/>
       <c r="AL33" s="14"/>
-      <c r="AM33" s="8"/>
+      <c r="AM33" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="AN33" s="8"/>
       <c r="AO33" s="8"/>
       <c r="AP33" s="14"/>
@@ -2109,11 +2113,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:V2"/>
     <mergeCell ref="W2:Z2"/>
     <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="AE2:AH2"/>
@@ -2124,6 +2123,11 @@
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="AY2:BB2"/>
     <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>